<commit_message>
Tidied up all variables and activities. Added a Throw business exception in case there are 11 players but they don't fit every position on board. Moved the SendFailureEmail part form Enough_Players_Exist workflow to Catch section in Main.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndreiHandrau\Documents\UiPath\Futbin_Best_11_Creation\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndreiHandrau\Documents\GitHub\Futbin_Best11Creation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F12EF1D-F25B-4BD9-8CB7-BB3636967DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5974400-3053-47BD-9217-C44207F0D30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -139,25 +139,44 @@
     <t>EmailReceiver</t>
   </si>
   <si>
+    <t>Not Enough Players</t>
+  </si>
+  <si>
+    <t>Need different criteria to choose players as current ones filter out too few players.</t>
+  </si>
+  <si>
+    <t>EmailBodyFailure</t>
+  </si>
+  <si>
+    <t>EmailSubjectFailure</t>
+  </si>
+  <si>
+    <t>EmailSubjectSuccess</t>
+  </si>
+  <si>
+    <t>Squad building successful</t>
+  </si>
+  <si>
     <t>handrauandrei@gmail.com</t>
   </si>
   <si>
-    <t>Not Enough Players</t>
-  </si>
-  <si>
-    <t>Need different criteria to choose players as current ones filter out too few players.</t>
-  </si>
-  <si>
-    <t>EmailBodyFailure</t>
-  </si>
-  <si>
-    <t>EmailSubjectFailure</t>
-  </si>
-  <si>
-    <t>EmailSubjectSuccess</t>
-  </si>
-  <si>
-    <t>Squad building successful</t>
+    <t>BuildFormationDelay</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This has been added to wait for website to load before the necessary item is being clicked on. Time is in </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>miliseconds</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -218,7 +237,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -229,6 +248,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -510,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -603,7 +624,7 @@
       <c r="A11" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="6" t="s">
         <v>20</v>
       </c>
     </row>
@@ -611,32 +632,43 @@
       <c r="A12" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>22</v>
+      <c r="B12" s="7" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17">
+        <v>2000</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -644,10 +676,9 @@
     <hyperlink ref="B5" r:id="rId1" xr:uid="{F5073E5D-0625-49FB-B98E-A31FC864FAE8}"/>
     <hyperlink ref="B6" r:id="rId2" xr:uid="{748453E7-6100-483F-9720-F5381EF105CD}"/>
     <hyperlink ref="B7" r:id="rId3" xr:uid="{6F955384-D7A6-4590-BAAD-9471BA4F9ACA}"/>
-    <hyperlink ref="B11" r:id="rId4" xr:uid="{72C35E6C-3072-4E0A-A635-CE1077CB06D5}"/>
-    <hyperlink ref="B12" r:id="rId5" xr:uid="{7FA78FAA-9971-4412-99C2-1F7E2F97749F}"/>
+    <hyperlink ref="B12" r:id="rId4" xr:uid="{BC0A2C1C-69BA-4AF5-B4BF-00DFED50047E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added bre text to config. Tidied up send email at end of try catch. Finished fix for element timeout in Futbin_ShowPlayers workflow
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndreiHandrau\Documents\GitHub\Futbin_Best11Creation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5974400-3053-47BD-9217-C44207F0D30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB5A50B0-E397-4852-95A0-A8EF3B7455B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -142,12 +142,6 @@
     <t>Not Enough Players</t>
   </si>
   <si>
-    <t>Need different criteria to choose players as current ones filter out too few players.</t>
-  </si>
-  <si>
-    <t>EmailBodyFailure</t>
-  </si>
-  <si>
     <t>EmailSubjectFailure</t>
   </si>
   <si>
@@ -163,20 +157,19 @@
     <t>BuildFormationDelay</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">This has been added to wait for website to load before the necessary item is being clicked on. Time is in </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>miliseconds</t>
-    </r>
+    <t>This is the value(in minutes for how long to wait to check if element has loaded</t>
+  </si>
+  <si>
+    <t>Error: Element loading time exceeded!</t>
+  </si>
+  <si>
+    <t>delayBRException</t>
+  </si>
+  <si>
+    <t>playernrBRException</t>
+  </si>
+  <si>
+    <t>Error: Not enough players to form a team!</t>
   </si>
 </sst>
 </file>
@@ -531,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -633,42 +626,50 @@
         <v>21</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
         <v>29</v>
       </c>
-      <c r="B17">
-        <v>2000</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>30</v>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>